<commit_message>
Se implemento las validaciones básicas para los informes post y adm
</commit_message>
<xml_diff>
--- a/app/tec/tec.xlsx
+++ b/app/tec/tec.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3798" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3798" uniqueCount="475">
   <si>
     <t>NO</t>
   </si>
@@ -1443,6 +1443,9 @@
   </si>
   <si>
     <t>1908010000731475_</t>
+  </si>
+  <si>
+    <t>Diagrama Call Center -&gt; Opciones de IVR</t>
   </si>
 </sst>
 </file>
@@ -4243,8 +4246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BO3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BZ30" sqref="BZ30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11827,7 +11830,7 @@
         <v>28</v>
       </c>
       <c r="BZ30" s="21" t="s">
-        <v>150</v>
+        <v>474</v>
       </c>
       <c r="CA30" s="21" t="s">
         <v>27</v>

</xml_diff>